<commit_message>
Complete point 2 and improve logisctic regression
</commit_message>
<xml_diff>
--- a/Diccionario_de_datos.xlsx
+++ b/Diccionario_de_datos.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camilo_\Documents\materias\BI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javier\Documents\code\BI\project1-text-analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37C5B742-3D67-41FF-BABC-6A3A1517EC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E895E52-299D-45DC-878A-4BC68F744A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11520" xr2:uid="{8CBC2610-D62D-42CB-B9EF-97DBB29590B6}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="14496" xr2:uid="{8CBC2610-D62D-42CB-B9EF-97DBB29590B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Diccionario_de_datos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,32 +47,31 @@
     <t>ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Identificador unico de la noticia </t>
-  </si>
-  <si>
     <t xml:space="preserve">Label </t>
   </si>
   <si>
     <t xml:space="preserve">Titulo </t>
   </si>
   <si>
-    <t>Titulo de la noticia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Descripción </t>
   </si>
   <si>
-    <t>Resumen de la noticia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fecha </t>
   </si>
   <si>
-    <t>Fechas en la que fue pulicada
-  cada notica hasta el dia de hoy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Etiqueta que indica si la notica es falsa(1) o verdadera (0) </t>
+    <t>Contiene el identificador del registro, sin embargo, todos los registros tienen la cadena ID.</t>
+  </si>
+  <si>
+    <t>Es la etiqueta del registro; 1 si el registro es una noticia falsa, 0 de lo contrario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corresponde al titulo de la noticia en español. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corresponde a la descripción o el cuerpo de la noticia en español. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Es la fecha en la que se publico la noticia, no hay registros de este año. Esta en formato día/mes/año. </t>
   </si>
 </sst>
 </file>
@@ -96,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -105,16 +104,100 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -123,13 +206,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,65 +563,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDCD24F-2143-4389-8E9F-43F948445200}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="2:3" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="2:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="8" spans="2:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>